<commit_message>
Algumas actualizacoes que fiz
Ipdates
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma doTrabalhos BD2.xlsx
+++ b/Documentos Base de dados/Cronograma doTrabalhos BD2.xlsx
@@ -289,6 +289,33 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -301,44 +328,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -616,7 +616,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,7 +627,7 @@
   <dimension ref="B3:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,12 +648,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="1" t="s">
         <v>22</v>
       </c>
@@ -698,48 +698,48 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="26">
         <v>44572</v>
       </c>
-      <c r="I4" s="19"/>
+      <c r="I4" s="27"/>
       <c r="J4" s="5">
         <v>44662</v>
       </c>
       <c r="K4" s="5">
         <v>44815</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21" t="s">
+      <c r="M4" s="19"/>
+      <c r="N4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="13" t="s">
+      <c r="O4" s="29"/>
+      <c r="P4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="15"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="24"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
+      <c r="B5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -758,10 +758,10 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -780,10 +780,10 @@
       </c>
     </row>
     <row r="7" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -802,10 +802,10 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -824,10 +824,10 @@
       </c>
     </row>
     <row r="9" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -868,12 +868,12 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -892,10 +892,10 @@
       </c>
     </row>
     <row r="12" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -914,10 +914,10 @@
       </c>
     </row>
     <row r="13" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -936,10 +936,10 @@
       </c>
     </row>
     <row r="14" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -958,10 +958,10 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
@@ -980,10 +980,10 @@
       </c>
     </row>
     <row r="16" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
@@ -1002,12 +1002,12 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1026,10 +1026,10 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1048,10 +1048,10 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -1070,10 +1070,10 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -1093,6 +1093,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="B17:B20"/>
@@ -1109,15 +1118,6 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacao da classe cliente
Actualizacoes Feitas a classe cliente para permitir a sua consulta
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma doTrabalhos BD2.xlsx
+++ b/Documentos Base de dados/Cronograma doTrabalhos BD2.xlsx
@@ -233,6 +233,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -248,23 +260,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,12 +571,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
@@ -621,40 +621,40 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="15">
         <v>44572</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="5">
         <v>44662</v>
       </c>
       <c r="K4" s="5">
         <v>44815</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="14" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="8" t="s">
+      <c r="O4" s="18"/>
+      <c r="P4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">

</xml_diff>